<commit_message>
Created Momentum strategy for sp500 tickers need to add hqm
</commit_message>
<xml_diff>
--- a/Trade_Details.xlsx
+++ b/Trade_Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivin/Desktop/Algorithmic_Trading_Bot_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309BB608-8497-6B46-9B88-90DAE2A91D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB51A6F-D340-5541-9F7C-57E3E11B6B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1900,7 +1900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A455" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>